<commit_message>
csv to pokemon json finished
</commit_message>
<xml_diff>
--- a/Code/03 IKT PYTHON/excelToPokemon/PokemonSet.xlsx
+++ b/Code/03 IKT PYTHON/excelToPokemon/PokemonSet.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adri2\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adri2\Desktop\Visual Studio Code\1IM-IKT\Code\03 IKT PYTHON\excelToPokemon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B49316A4-9AE6-4C08-841B-94DCE57AE401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E9FF6678-C903-45FB-B67F-DC43512A4314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="17040" windowHeight="12336" activeTab="1" xr2:uid="{A21DBED3-E6F7-4655-A3B1-386E99579C25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" xr2:uid="{A21DBED3-E6F7-4655-A3B1-386E99579C25}"/>
   </bookViews>
   <sheets>
-    <sheet name="PokemonSet" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -249,168 +249,219 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
-  <si>
-    <t>Number</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+  <si>
+    <t>baseSetId</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>subname</t>
+  </si>
+  <si>
+    <t>prevolveName</t>
+  </si>
+  <si>
+    <t>hitpoints</t>
+  </si>
+  <si>
+    <t>supertypeId</t>
+  </si>
+  <si>
+    <t>typeId</t>
+  </si>
+  <si>
+    <t>subtypeId</t>
+  </si>
+  <si>
+    <t>variationId</t>
+  </si>
+  <si>
+    <t>rarityId</t>
+  </si>
+  <si>
+    <t>dexNumber</t>
+  </si>
+  <si>
+    <t>dexCategory</t>
+  </si>
+  <si>
+    <t>dexHeight</t>
+  </si>
+  <si>
+    <t>dexWeight</t>
+  </si>
+  <si>
+    <t>illustrator</t>
+  </si>
+  <si>
+    <t>cardNumber</t>
+  </si>
+  <si>
+    <t>totalInSet</t>
+  </si>
+  <si>
+    <t>rarityIconId</t>
+  </si>
+  <si>
+    <t>Sword Shield</t>
+  </si>
+  <si>
+    <t>Cynthia</t>
+  </si>
+  <si>
+    <t>Marnie</t>
+  </si>
+  <si>
+    <t>Pokemon</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Trainer</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Nemona</t>
+  </si>
+  <si>
+    <t>Lillie</t>
+  </si>
+  <si>
+    <t>Supertype</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
+    <t>Subtype</t>
+  </si>
+  <si>
+    <t>Variation</t>
+  </si>
+  <si>
     <t>Rarity</t>
   </si>
   <si>
-    <t>Subtype</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>Rarity Icon</t>
+  </si>
+  <si>
+    <t>Sun Moon</t>
+  </si>
+  <si>
+    <t>Stage 1</t>
+  </si>
+  <si>
+    <t>Dynamax</t>
   </si>
   <si>
     <t>Promo</t>
   </si>
   <si>
+    <t>Scarlet Violet</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Stage 2</t>
+  </si>
+  <si>
+    <t>Gigantamax</t>
+  </si>
+  <si>
+    <t>Full Art</t>
+  </si>
+  <si>
+    <t>XY BW</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Golden Full Art</t>
+  </si>
+  <si>
+    <t>Vmax</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>Rainbow</t>
+  </si>
+  <si>
+    <t>VStar</t>
+  </si>
+  <si>
+    <t>ex</t>
+  </si>
+  <si>
+    <t>gx (Basic)</t>
+  </si>
+  <si>
+    <t>Ultra Beast</t>
+  </si>
+  <si>
+    <t>gx (Stage 1)</t>
+  </si>
+  <si>
+    <t>Prism Star</t>
+  </si>
+  <si>
+    <t>gx (Stage 2)</t>
+  </si>
+  <si>
+    <t>Tag Team</t>
+  </si>
+  <si>
     <t>Character Rare</t>
   </si>
   <si>
-    <t>Basic</t>
-  </si>
-  <si>
-    <t>Stage 1</t>
-  </si>
-  <si>
-    <t>Stage 2</t>
+    <t>gx (Tag Team)</t>
+  </si>
+  <si>
+    <t>Gold Star</t>
   </si>
   <si>
     <t>Lv. X</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Vmax</t>
-  </si>
-  <si>
-    <t>VStar</t>
-  </si>
-  <si>
-    <t>Variation</t>
-  </si>
-  <si>
-    <t>Light</t>
-  </si>
-  <si>
-    <t>Dark</t>
-  </si>
-  <si>
-    <t>ex</t>
-  </si>
-  <si>
-    <t>Rarity Icon</t>
-  </si>
-  <si>
-    <t>Cynthia</t>
-  </si>
-  <si>
-    <t>Trainer</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Pokemon</t>
-  </si>
-  <si>
-    <t>Nemona</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>subname</t>
-  </si>
-  <si>
-    <t>hitpoints</t>
-  </si>
-  <si>
-    <t>typeId</t>
-  </si>
-  <si>
-    <t>subtypeId</t>
+    <t>Tera</t>
+  </si>
+  <si>
+    <t>ex (Basic)</t>
+  </si>
+  <si>
+    <t>Fossil</t>
+  </si>
+  <si>
+    <t>ex (Stage 1)</t>
   </si>
   <si>
     <t>Radiant</t>
   </si>
   <si>
-    <t>Gold Star</t>
-  </si>
-  <si>
-    <t>variationId</t>
-  </si>
-  <si>
-    <t>rarityIconId</t>
-  </si>
-  <si>
-    <t>cardNumber</t>
-  </si>
-  <si>
-    <t>totalInSet</t>
-  </si>
-  <si>
-    <t>illustrator</t>
-  </si>
-  <si>
-    <t>dexNumber</t>
-  </si>
-  <si>
-    <t>dexCategory</t>
-  </si>
-  <si>
-    <t>dexHeight</t>
-  </si>
-  <si>
-    <t>dexWeight</t>
-  </si>
-  <si>
-    <t>gx (Basic)</t>
-  </si>
-  <si>
-    <t>gx (Stage 1)</t>
-  </si>
-  <si>
-    <t>gx (Stage 2)</t>
-  </si>
-  <si>
-    <t>gx (Tag Team)</t>
-  </si>
-  <si>
-    <t>ex (Basic)</t>
-  </si>
-  <si>
-    <t>ex (Stage 1)</t>
+    <t>Golden</t>
   </si>
   <si>
     <t>ex (Stage 2)</t>
   </si>
   <si>
-    <t>rarityId</t>
-  </si>
-  <si>
-    <t>Golden</t>
-  </si>
-  <si>
-    <t>Ultra Beast</t>
-  </si>
-  <si>
-    <t>Prism Star</t>
-  </si>
-  <si>
-    <t>Full Art</t>
-  </si>
-  <si>
-    <t>var 7</t>
-  </si>
-  <si>
-    <t>var 6</t>
+    <t>Team Flare</t>
+  </si>
+  <si>
+    <t>Team Plasma</t>
   </si>
 </sst>
 </file>
@@ -426,7 +477,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,12 +502,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -470,20 +515,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,9 +726,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -722,7 +766,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -828,7 +872,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -970,7 +1014,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -978,205 +1022,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A575EC3D-1A30-465C-AAFE-3C46B3AC68AE}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2">
         <v>100</v>
       </c>
-      <c r="D2" s="2" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
       </c>
       <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
-        <v>21</v>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="M2" s="2">
         <v>1</v>
       </c>
       <c r="N2" s="2">
-        <f ca="1">COUNT(N:N)</f>
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>COUNT(N:N)</f>
         <v>2</v>
       </c>
-      <c r="O2" s="5" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R2" s="4" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2">
-        <v>200</v>
-      </c>
-      <c r="D3" s="2" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="K3" s="2">
         <v>2</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="L3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="2">
         <v>5</v>
       </c>
-      <c r="K3" s="2">
+      <c r="N3" s="2">
         <v>5</v>
       </c>
-      <c r="L3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="2">
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2">
         <v>2</v>
       </c>
-      <c r="N3" s="2">
-        <f ca="1">COUNT(N:N)</f>
+      <c r="Q3" s="2">
+        <f>COUNT(N:N)</f>
         <v>2</v>
       </c>
-      <c r="O3" s="5" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="R3" s="4" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3EB64F1F-1716-412A-8FBF-48E8CE5EB592}">
-          <x14:formula1>
-            <xm:f>Data!$E$3:$E$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F3</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED17186D-5F37-4B1B-92B1-089716F24948}">
           <x14:formula1>
             <xm:f>Data!$C$3:$C$13</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D3</xm:sqref>
+          <xm:sqref>G2:G3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2EB79516-DA1C-4C39-A9B8-CF1C3ACB1E80}">
           <x14:formula1>
             <xm:f>Data!$D$3:$D$16</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E3</xm:sqref>
+          <xm:sqref>H2:H3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BEDC73FB-C3C1-44CA-8CB7-6D4006B0DB43}">
           <x14:formula1>
             <xm:f>Data!$G$3:$G$11</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O3</xm:sqref>
+          <xm:sqref>R2:R3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{116DCF58-E861-4C85-AA7D-2D38B9980076}">
           <x14:formula1>
             <xm:f>Data!$J$8:$J$10</xm:f>
           </x14:formula1>
-          <xm:sqref>F13:F15 H6:H12 G2:G4</xm:sqref>
+          <xm:sqref>F13:F15 H6:H12 J4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{576CE5B6-CA9E-447C-8BC8-905D6CCDA0AB}">
+          <x14:formula1>
+            <xm:f>Data!$B$3:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3A2DB556-8394-4A37-9C78-0C9DC11E295B}">
+          <x14:formula1>
+            <xm:f>Data!$A$3:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3EB64F1F-1716-412A-8FBF-48E8CE5EB592}">
+          <x14:formula1>
+            <xm:f>Data!$E$3:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>I3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4FEEC8B-E122-4CED-B3FE-76600AA719E8}">
+          <x14:formula1>
+            <xm:f>Data!$E$3:$E$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79ADF293-0828-4A6C-B735-A349095D513E}">
+          <x14:formula1>
+            <xm:f>Data!$F$3:$F$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1186,237 +1293,413 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F2589E-4C76-4C19-890B-A05C2CDD6FB9}">
-  <dimension ref="B2:J17"/>
+  <dimension ref="A2:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="6.21875" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="6" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="3" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="3" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="3" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="L6" s="3" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="3" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="3" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="3" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="L8" s="3" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="e" vm="16">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="3" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9" s="3" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="e" vm="17">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="3" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10" s="3" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="e" vm="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="3" t="e" vm="19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11" s="3" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="e" vm="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+      <c r="L12" s="3" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+      <c r="L13" s="3" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14" s="3" t="e" vm="19">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="L22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>8</v>
+      </c>
+      <c r="L27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>12</v>
+      </c>
+      <c r="L31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>13</v>
+      </c>
+      <c r="L32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K33">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="4" t="e" vm="6">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="e" vm="7">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="4" t="e" vm="8">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="e" vm="9">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="4" t="e" vm="10">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="e" vm="11">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="4" t="e" vm="12">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="4" t="e" vm="13">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="2" t="e" vm="14">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="4" t="e" vm="15">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="e" vm="16">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="4" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="e" vm="17">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="4" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I10">
-        <v>8</v>
-      </c>
-      <c r="J10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="e" vm="18">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="4" t="e" vm="19">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I11">
-        <v>12</v>
-      </c>
-      <c r="J11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="e" vm="20">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="I12" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="I13" t="s">
-        <v>52</v>
-      </c>
-      <c r="J13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="I14">
-        <v>2</v>
-      </c>
-      <c r="J14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G17" s="3"/>
+      <c r="L33" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J10" xr:uid="{D8A87763-9211-4E9C-B048-4840866FDF20}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8 J22 L27 L20 F3:F4 F11" xr:uid="{D8A87763-9211-4E9C-B048-4840866FDF20}">
       <formula1>$J$8:$J$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -1425,6 +1708,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b1227f61-4b01-4b9a-91d2-bad7f317c526" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DF963FFE007BF54987A8A3EBC492B25A" ma:contentTypeVersion="16" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="e10de3fe57c438606a4aa3a270bed9d9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b1227f61-4b01-4b9a-91d2-bad7f317c526" xmlns:ns4="f39e6ce4-1b24-43f0-ac3a-8251e17daebe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f26e344238766926d45c3629394d15e" ns3:_="" ns4:_="">
     <xsd:import namespace="b1227f61-4b01-4b9a-91d2-bad7f317c526"/>
@@ -1663,24 +1963,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA826C7-F3C0-4F3D-A04A-3D59CB43E679}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b1227f61-4b01-4b9a-91d2-bad7f317c526" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D3C3A23-D496-45CF-B297-111F402C5563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b1227f61-4b01-4b9a-91d2-bad7f317c526"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D009B73D-034C-41D9-BAEE-9820048FE077}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1697,18 +1998,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA826C7-F3C0-4F3D-A04A-3D59CB43E679}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D3C3A23-D496-45CF-B297-111F402C5563}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
 </file>
</xml_diff>